<commit_message>
performed a clean up
</commit_message>
<xml_diff>
--- a/KS2/Year-3.xlsx
+++ b/KS2/Year-3.xlsx
@@ -366,9 +366,6 @@
     <t>Learners should identify and name the objects they will need for a project
 Learners should implement their algorithm as code
 Learners should relate a task description to a design</t>
-  </si>
-  <si>
-    <t>Introduction of Digital Safety</t>
   </si>
   <si>
     <t>Learners should define hacking in the context of Digital safety
@@ -617,6 +614,9 @@
   </si>
   <si>
     <t>To explain how a computer network can be used To share information</t>
+  </si>
+  <si>
+    <t>Introduction to Digital Safety</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1024,23 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1298,8 +1314,8 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="38.1" customHeight="1"/>
@@ -1380,7 +1396,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>78</v>
@@ -1401,7 +1417,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>52</v>
@@ -1421,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>78</v>
@@ -1442,7 +1458,7 @@
         <v>5</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>53</v>
@@ -1462,7 +1478,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>78</v>
@@ -1483,7 +1499,7 @@
         <v>7</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>54</v>
@@ -1503,7 +1519,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>48</v>
@@ -1524,7 +1540,7 @@
         <v>14</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>64</v>
@@ -1544,7 +1560,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>48</v>
@@ -1565,7 +1581,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>55</v>
@@ -1585,7 +1601,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>48</v>
@@ -1606,7 +1622,7 @@
         <v>18</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>56</v>
@@ -1626,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>48</v>
@@ -1647,7 +1663,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>62</v>
@@ -1667,7 +1683,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>48</v>
@@ -1688,7 +1704,7 @@
         <v>22</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>61</v>
@@ -1708,7 +1724,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>48</v>
@@ -1729,7 +1745,7 @@
         <v>24</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>60</v>
@@ -1749,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>78</v>
@@ -1767,10 +1783,10 @@
         <v>1</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J12" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>57</v>
@@ -1790,7 +1806,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>78</v>
@@ -1811,7 +1827,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>58</v>
@@ -1831,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>78</v>
@@ -1852,7 +1868,7 @@
         <v>12</v>
       </c>
       <c r="J14" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K14" s="11" t="s">
         <v>59</v>
@@ -1872,13 +1888,13 @@
         <v>3</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>79</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="F15" s="27">
         <v>1</v>
@@ -1893,13 +1909,13 @@
         <v>80</v>
       </c>
       <c r="J15" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K15" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L15" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M15" s="30"/>
     </row>
@@ -1911,13 +1927,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>79</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="F16" s="27">
         <v>2</v>
@@ -1932,13 +1948,13 @@
         <v>82</v>
       </c>
       <c r="J16" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K16" s="29" t="s">
         <v>81</v>
       </c>
       <c r="L16" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M16" s="30"/>
     </row>
@@ -1950,13 +1966,13 @@
         <v>3</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>79</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="F17" s="27">
         <v>3</v>
@@ -1971,10 +1987,10 @@
         <v>83</v>
       </c>
       <c r="J17" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K17" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L17" s="29" t="s">
         <v>84</v>
@@ -1989,7 +2005,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>50</v>
@@ -2010,7 +2026,7 @@
         <v>26</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>85</v>
@@ -2030,7 +2046,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>50</v>
@@ -2051,7 +2067,7 @@
         <v>28</v>
       </c>
       <c r="J19" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>86</v>
@@ -2071,7 +2087,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>50</v>
@@ -2092,7 +2108,7 @@
         <v>30</v>
       </c>
       <c r="J20" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K20" s="11" t="s">
         <v>87</v>
@@ -2112,7 +2128,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>50</v>
@@ -2133,7 +2149,7 @@
         <v>32</v>
       </c>
       <c r="J21" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>65</v>
@@ -2153,7 +2169,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>50</v>
@@ -2174,7 +2190,7 @@
         <v>34</v>
       </c>
       <c r="J22" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>66</v>
@@ -2194,7 +2210,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>50</v>
@@ -2215,7 +2231,7 @@
         <v>35</v>
       </c>
       <c r="J23" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>69</v>
@@ -2235,7 +2251,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>50</v>
@@ -2256,7 +2272,7 @@
         <v>71</v>
       </c>
       <c r="J24" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>73</v>
@@ -2276,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>50</v>
@@ -2297,7 +2313,7 @@
         <v>72</v>
       </c>
       <c r="J25" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>74</v>
@@ -2317,7 +2333,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>50</v>
@@ -2338,7 +2354,7 @@
         <v>36</v>
       </c>
       <c r="J26" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K26" s="11" t="s">
         <v>76</v>
@@ -2359,42 +2375,42 @@
     <filterColumn colId="9"/>
   </autoFilter>
   <conditionalFormatting sqref="M3:M26 B3:L5 B18:L20">
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>$M3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M26 B3:L5 B18:L20">
-    <cfRule type="expression" dxfId="6" priority="17">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>$M3=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:L17">
-    <cfRule type="expression" dxfId="5" priority="19">
+    <cfRule type="expression" dxfId="7" priority="19">
       <formula>$M6=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:L17">
-    <cfRule type="expression" dxfId="4" priority="21">
+    <cfRule type="expression" dxfId="6" priority="21">
       <formula>$M6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:L11">
-    <cfRule type="expression" dxfId="3" priority="23">
+    <cfRule type="expression" dxfId="5" priority="23">
       <formula>$M9=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:L11">
-    <cfRule type="expression" dxfId="2" priority="25">
+    <cfRule type="expression" dxfId="4" priority="25">
       <formula>$M9=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:L26">
-    <cfRule type="expression" dxfId="1" priority="36">
+    <cfRule type="expression" dxfId="3" priority="36">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:L26">
-    <cfRule type="expression" dxfId="0" priority="37">
+    <cfRule type="expression" dxfId="2" priority="37">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>